<commit_message>
Adicionar Coluna Historico nos Ranking
</commit_message>
<xml_diff>
--- a/ranking.xlsx
+++ b/ranking.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio Felipe\Local Sites\cenp\app\public\wp-content\plugins\cenp-meios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caiof\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="RANKING" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>POSICAO</t>
   </si>
@@ -35,15 +35,29 @@
   <si>
     <t>UF</t>
   </si>
+  <si>
+    <t>POSICAO_ANTERIOR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,11 +83,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,1309 +383,1524 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C257"/>
+  <dimension ref="A1:D256"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2"/>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
       <c r="B2"/>
-      <c r="C2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
       <c r="B3"/>
-      <c r="C3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
       <c r="B4"/>
-      <c r="C4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
       <c r="B5"/>
-      <c r="C5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
       <c r="B6"/>
-      <c r="C6"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
       <c r="B7"/>
-      <c r="C7"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
       <c r="B8"/>
-      <c r="C8"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
       <c r="B9"/>
-      <c r="C9"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
       <c r="B10"/>
-      <c r="C10"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
       <c r="B11"/>
-      <c r="C11"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
       <c r="B12"/>
-      <c r="C12"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
       <c r="B13"/>
-      <c r="C13"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
       <c r="B14"/>
-      <c r="C14"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
       <c r="B15"/>
-      <c r="C15"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
       <c r="B16"/>
-      <c r="C16"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
       <c r="B17"/>
-      <c r="C17"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
       <c r="B18"/>
-      <c r="C18"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
       <c r="B19"/>
-      <c r="C19"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
       <c r="B20"/>
-      <c r="C20"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
       <c r="B21"/>
-      <c r="C21"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
       <c r="B22"/>
-      <c r="C22"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
       <c r="B23"/>
-      <c r="C23"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
       <c r="B24"/>
-      <c r="C24"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
       <c r="B25"/>
-      <c r="C25"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
       <c r="B26"/>
-      <c r="C26"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
       <c r="B27"/>
-      <c r="C27"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
       <c r="B28"/>
-      <c r="C28"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
       <c r="B29"/>
-      <c r="C29"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
       <c r="B30"/>
-      <c r="C30"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
       <c r="B31"/>
-      <c r="C31"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
       <c r="B32"/>
-      <c r="C32"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
       <c r="B33"/>
-      <c r="C33"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
       <c r="B34"/>
-      <c r="C34"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
       <c r="B35"/>
-      <c r="C35"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
       <c r="B36"/>
-      <c r="C36"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
       <c r="B37"/>
-      <c r="C37"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
       <c r="B38"/>
-      <c r="C38"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
       <c r="B39"/>
-      <c r="C39"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
       <c r="B40"/>
-      <c r="C40"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
       <c r="B41"/>
-      <c r="C41"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="7"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
       <c r="B42"/>
-      <c r="C42"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="7"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
       <c r="B43"/>
-      <c r="C43"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
       <c r="B44"/>
-      <c r="C44"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
       <c r="B45"/>
-      <c r="C45"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
       <c r="B46"/>
-      <c r="C46"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
       <c r="B47"/>
-      <c r="C47"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="7"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
       <c r="B48"/>
-      <c r="C48"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
       <c r="B49"/>
-      <c r="C49"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="7"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
       <c r="B50"/>
-      <c r="C50"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="7"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
       <c r="B51"/>
-      <c r="C51"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
       <c r="B52"/>
-      <c r="C52"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
       <c r="B53"/>
-      <c r="C53"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
       <c r="B54"/>
-      <c r="C54"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="7"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
       <c r="B55"/>
-      <c r="C55"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="7"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
       <c r="B56"/>
-      <c r="C56"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="7"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
       <c r="B57"/>
-      <c r="C57"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
       <c r="B58"/>
-      <c r="C58"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="7"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
       <c r="B59"/>
-      <c r="C59"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="7"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
       <c r="B60"/>
-      <c r="C60"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="7"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
       <c r="B61"/>
-      <c r="C61"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="7"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
       <c r="B62"/>
-      <c r="C62"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="7"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
       <c r="B63"/>
-      <c r="C63"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="7"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
       <c r="B64"/>
-      <c r="C64"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
       <c r="B65"/>
-      <c r="C65"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="7"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
       <c r="B66"/>
-      <c r="C66"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="7"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
       <c r="B67"/>
-      <c r="C67"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="7"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
       <c r="B68"/>
-      <c r="C68"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="7"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="5"/>
       <c r="B69"/>
-      <c r="C69"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="7"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
       <c r="B70"/>
-      <c r="C70"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="7"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
       <c r="B71"/>
-      <c r="C71"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="7"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
       <c r="B72"/>
-      <c r="C72"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="7"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
       <c r="B73"/>
-      <c r="C73"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="7"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
       <c r="B74"/>
-      <c r="C74"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="7"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
       <c r="B75"/>
-      <c r="C75"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="7"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
       <c r="B76"/>
-      <c r="C76"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="7"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="5"/>
       <c r="B77"/>
-      <c r="C77"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="7"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
       <c r="B78"/>
-      <c r="C78"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="7"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="5"/>
       <c r="B79"/>
-      <c r="C79"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="7"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
       <c r="B80"/>
-      <c r="C80"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="7"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
       <c r="B81"/>
-      <c r="C81"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="7"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
       <c r="B82"/>
-      <c r="C82"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="7"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
       <c r="B83"/>
-      <c r="C83"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="7"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
       <c r="B84"/>
-      <c r="C84"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="7"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
       <c r="B85"/>
-      <c r="C85"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="7"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
       <c r="B86"/>
-      <c r="C86"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="7"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
       <c r="B87"/>
-      <c r="C87"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="7"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
       <c r="B88"/>
-      <c r="C88"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="7"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
       <c r="B89"/>
-      <c r="C89"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="7"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
       <c r="B90"/>
-      <c r="C90"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="7"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="5"/>
       <c r="B91"/>
-      <c r="C91"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="7"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="5"/>
       <c r="B92"/>
-      <c r="C92"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="7"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="5"/>
       <c r="B93"/>
-      <c r="C93"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="7"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="5"/>
       <c r="B94"/>
-      <c r="C94"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="7"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
       <c r="B95"/>
-      <c r="C95"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="7"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
       <c r="B96"/>
-      <c r="C96"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="7"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="5"/>
       <c r="B97"/>
-      <c r="C97"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="7"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="5"/>
       <c r="B98"/>
-      <c r="C98"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="7"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="5"/>
       <c r="B99"/>
-      <c r="C99"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="7"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="5"/>
       <c r="B100"/>
-      <c r="C100"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="7"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="5"/>
       <c r="B101"/>
-      <c r="C101"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="7"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="5"/>
       <c r="B102"/>
-      <c r="C102"/>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="7"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="5"/>
       <c r="B103"/>
-      <c r="C103"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="7"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="5"/>
       <c r="B104"/>
-      <c r="C104"/>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="7"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="5"/>
       <c r="B105"/>
-      <c r="C105"/>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="7"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="5"/>
       <c r="B106"/>
-      <c r="C106"/>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="7"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="5"/>
       <c r="B107"/>
-      <c r="C107"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="7"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="5"/>
       <c r="B108"/>
-      <c r="C108"/>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="7"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="5"/>
       <c r="B109"/>
-      <c r="C109"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="7"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="5"/>
       <c r="B110"/>
-      <c r="C110"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="7"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="5"/>
       <c r="B111"/>
-      <c r="C111"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="7"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="5"/>
       <c r="B112"/>
-      <c r="C112"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="7"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="5"/>
       <c r="B113"/>
-      <c r="C113"/>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="7"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="5"/>
       <c r="B114"/>
-      <c r="C114"/>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="7"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="5"/>
       <c r="B115"/>
-      <c r="C115"/>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="7"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="5"/>
       <c r="B116"/>
-      <c r="C116"/>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="7"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="5"/>
       <c r="B117"/>
-      <c r="C117"/>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="7"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="5"/>
       <c r="B118"/>
-      <c r="C118"/>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="7"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="5"/>
       <c r="B119"/>
-      <c r="C119"/>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="7"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="5"/>
       <c r="B120"/>
-      <c r="C120"/>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="7"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="5"/>
       <c r="B121"/>
-      <c r="C121"/>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122"/>
+      <c r="C121" s="5"/>
+      <c r="D121" s="7"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="5"/>
       <c r="B122"/>
-      <c r="C122"/>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="7"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="5"/>
       <c r="B123"/>
-      <c r="C123"/>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="7"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="5"/>
       <c r="B124"/>
-      <c r="C124"/>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125"/>
+      <c r="C124" s="5"/>
+      <c r="D124" s="7"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="5"/>
       <c r="B125"/>
-      <c r="C125"/>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="7"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="5"/>
       <c r="B126"/>
-      <c r="C126"/>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="7"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="5"/>
       <c r="B127"/>
-      <c r="C127"/>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="7"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="5"/>
       <c r="B128"/>
-      <c r="C128"/>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="7"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="5"/>
       <c r="B129"/>
-      <c r="C129"/>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="7"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="5"/>
       <c r="B130"/>
-      <c r="C130"/>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="7"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="5"/>
       <c r="B131"/>
-      <c r="C131"/>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="7"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="5"/>
       <c r="B132"/>
-      <c r="C132"/>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="7"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="5"/>
       <c r="B133"/>
-      <c r="C133"/>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134"/>
+      <c r="C133" s="5"/>
+      <c r="D133" s="7"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="5"/>
       <c r="B134"/>
-      <c r="C134"/>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="7"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="5"/>
       <c r="B135"/>
-      <c r="C135"/>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="7"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="5"/>
       <c r="B136"/>
-      <c r="C136"/>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="7"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="5"/>
       <c r="B137"/>
-      <c r="C137"/>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="7"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="5"/>
       <c r="B138"/>
-      <c r="C138"/>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="7"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="5"/>
       <c r="B139"/>
-      <c r="C139"/>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="7"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="5"/>
       <c r="B140"/>
-      <c r="C140"/>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="7"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="5"/>
       <c r="B141"/>
-      <c r="C141"/>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="7"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="5"/>
       <c r="B142"/>
-      <c r="C142"/>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="7"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="5"/>
       <c r="B143"/>
-      <c r="C143"/>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="7"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="5"/>
       <c r="B144"/>
-      <c r="C144"/>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145"/>
+      <c r="C144" s="5"/>
+      <c r="D144" s="7"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="5"/>
       <c r="B145"/>
-      <c r="C145"/>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146"/>
+      <c r="C145" s="5"/>
+      <c r="D145" s="7"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="5"/>
       <c r="B146"/>
-      <c r="C146"/>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="7"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="5"/>
       <c r="B147"/>
-      <c r="C147"/>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="7"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="5"/>
       <c r="B148"/>
-      <c r="C148"/>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149"/>
+      <c r="C148" s="5"/>
+      <c r="D148" s="7"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="5"/>
       <c r="B149"/>
-      <c r="C149"/>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="7"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="5"/>
       <c r="B150"/>
-      <c r="C150"/>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151"/>
+      <c r="C150" s="5"/>
+      <c r="D150" s="7"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="5"/>
       <c r="B151"/>
-      <c r="C151"/>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152"/>
+      <c r="C151" s="5"/>
+      <c r="D151" s="7"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="5"/>
       <c r="B152"/>
-      <c r="C152"/>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153"/>
+      <c r="C152" s="5"/>
+      <c r="D152" s="7"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="5"/>
       <c r="B153"/>
-      <c r="C153"/>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154"/>
+      <c r="C153" s="5"/>
+      <c r="D153" s="7"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="5"/>
       <c r="B154"/>
-      <c r="C154"/>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155"/>
+      <c r="C154" s="5"/>
+      <c r="D154" s="7"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="5"/>
       <c r="B155"/>
-      <c r="C155"/>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156"/>
+      <c r="C155" s="5"/>
+      <c r="D155" s="7"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="5"/>
       <c r="B156"/>
-      <c r="C156"/>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157"/>
+      <c r="C156" s="5"/>
+      <c r="D156" s="7"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="5"/>
       <c r="B157"/>
-      <c r="C157"/>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158"/>
+      <c r="C157" s="5"/>
+      <c r="D157" s="7"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="5"/>
       <c r="B158"/>
-      <c r="C158"/>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159"/>
+      <c r="C158" s="5"/>
+      <c r="D158" s="7"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="5"/>
       <c r="B159"/>
-      <c r="C159"/>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160"/>
+      <c r="C159" s="5"/>
+      <c r="D159" s="7"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="5"/>
       <c r="B160"/>
-      <c r="C160"/>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161"/>
+      <c r="C160" s="5"/>
+      <c r="D160" s="7"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="5"/>
       <c r="B161"/>
-      <c r="C161"/>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="7"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="5"/>
       <c r="B162"/>
-      <c r="C162"/>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163"/>
+      <c r="C162" s="5"/>
+      <c r="D162" s="7"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="5"/>
       <c r="B163"/>
-      <c r="C163"/>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="7"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="5"/>
       <c r="B164"/>
-      <c r="C164"/>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="7"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="5"/>
       <c r="B165"/>
-      <c r="C165"/>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166"/>
+      <c r="C165" s="5"/>
+      <c r="D165" s="7"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="5"/>
       <c r="B166"/>
-      <c r="C166"/>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167"/>
+      <c r="C166" s="5"/>
+      <c r="D166" s="7"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="5"/>
       <c r="B167"/>
-      <c r="C167"/>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168"/>
+      <c r="C167" s="5"/>
+      <c r="D167" s="7"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="5"/>
       <c r="B168"/>
-      <c r="C168"/>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169"/>
+      <c r="C168" s="5"/>
+      <c r="D168" s="7"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="5"/>
       <c r="B169"/>
-      <c r="C169"/>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170"/>
+      <c r="C169" s="5"/>
+      <c r="D169" s="7"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="5"/>
       <c r="B170"/>
-      <c r="C170"/>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171"/>
+      <c r="C170" s="5"/>
+      <c r="D170" s="7"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="5"/>
       <c r="B171"/>
-      <c r="C171"/>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172"/>
+      <c r="C171" s="5"/>
+      <c r="D171" s="7"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="5"/>
       <c r="B172"/>
-      <c r="C172"/>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173"/>
+      <c r="C172" s="5"/>
+      <c r="D172" s="7"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="5"/>
       <c r="B173"/>
-      <c r="C173"/>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174"/>
+      <c r="C173" s="5"/>
+      <c r="D173" s="7"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="5"/>
       <c r="B174"/>
-      <c r="C174"/>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175"/>
+      <c r="C174" s="5"/>
+      <c r="D174" s="7"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="5"/>
       <c r="B175"/>
-      <c r="C175"/>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176"/>
+      <c r="C175" s="5"/>
+      <c r="D175" s="7"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="5"/>
       <c r="B176"/>
-      <c r="C176"/>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177"/>
+      <c r="C176" s="5"/>
+      <c r="D176" s="7"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="5"/>
       <c r="B177"/>
-      <c r="C177"/>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178"/>
+      <c r="C177" s="5"/>
+      <c r="D177" s="7"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="5"/>
       <c r="B178"/>
-      <c r="C178"/>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179"/>
+      <c r="C178" s="5"/>
+      <c r="D178" s="7"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="5"/>
       <c r="B179"/>
-      <c r="C179"/>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180"/>
+      <c r="C179" s="5"/>
+      <c r="D179" s="7"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="5"/>
       <c r="B180"/>
-      <c r="C180"/>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181"/>
+      <c r="C180" s="5"/>
+      <c r="D180" s="7"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="5"/>
       <c r="B181"/>
-      <c r="C181"/>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182"/>
+      <c r="C181" s="5"/>
+      <c r="D181" s="7"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="5"/>
       <c r="B182"/>
-      <c r="C182"/>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183"/>
+      <c r="C182" s="5"/>
+      <c r="D182" s="7"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="5"/>
       <c r="B183"/>
-      <c r="C183"/>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184"/>
+      <c r="C183" s="5"/>
+      <c r="D183" s="7"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="5"/>
       <c r="B184"/>
-      <c r="C184"/>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185"/>
+      <c r="C184" s="5"/>
+      <c r="D184" s="7"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="5"/>
       <c r="B185"/>
-      <c r="C185"/>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186"/>
+      <c r="C185" s="5"/>
+      <c r="D185" s="7"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="5"/>
       <c r="B186"/>
-      <c r="C186"/>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187"/>
+      <c r="C186" s="5"/>
+      <c r="D186" s="7"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="5"/>
       <c r="B187"/>
-      <c r="C187"/>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188"/>
+      <c r="C187" s="5"/>
+      <c r="D187" s="7"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="5"/>
       <c r="B188"/>
-      <c r="C188"/>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189"/>
+      <c r="C188" s="5"/>
+      <c r="D188" s="7"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="5"/>
       <c r="B189"/>
-      <c r="C189"/>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190"/>
+      <c r="C189" s="5"/>
+      <c r="D189" s="7"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="5"/>
       <c r="B190"/>
-      <c r="C190"/>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191"/>
+      <c r="C190" s="5"/>
+      <c r="D190" s="7"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="5"/>
       <c r="B191"/>
-      <c r="C191"/>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192"/>
+      <c r="C191" s="5"/>
+      <c r="D191" s="7"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="5"/>
       <c r="B192"/>
-      <c r="C192"/>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193"/>
+      <c r="C192" s="5"/>
+      <c r="D192" s="7"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="5"/>
       <c r="B193"/>
-      <c r="C193"/>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194"/>
+      <c r="C193" s="5"/>
+      <c r="D193" s="7"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="5"/>
       <c r="B194"/>
-      <c r="C194"/>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195"/>
+      <c r="C194" s="5"/>
+      <c r="D194" s="7"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="5"/>
       <c r="B195"/>
-      <c r="C195"/>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196"/>
+      <c r="C195" s="5"/>
+      <c r="D195" s="7"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="5"/>
       <c r="B196"/>
-      <c r="C196"/>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197"/>
+      <c r="C196" s="5"/>
+      <c r="D196" s="7"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="5"/>
       <c r="B197"/>
-      <c r="C197"/>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198"/>
+      <c r="C197" s="5"/>
+      <c r="D197" s="7"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="5"/>
       <c r="B198"/>
-      <c r="C198"/>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199"/>
+      <c r="C198" s="5"/>
+      <c r="D198" s="7"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="5"/>
       <c r="B199"/>
-      <c r="C199"/>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200"/>
+      <c r="C199" s="5"/>
+      <c r="D199" s="7"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="5"/>
       <c r="B200"/>
-      <c r="C200"/>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201"/>
+      <c r="C200" s="5"/>
+      <c r="D200" s="7"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="5"/>
       <c r="B201"/>
-      <c r="C201"/>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202"/>
+      <c r="C201" s="5"/>
+      <c r="D201" s="7"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="5"/>
       <c r="B202"/>
-      <c r="C202"/>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203"/>
+      <c r="C202" s="5"/>
+      <c r="D202" s="7"/>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="5"/>
       <c r="B203"/>
-      <c r="C203"/>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204"/>
+      <c r="C203" s="5"/>
+      <c r="D203" s="7"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="5"/>
       <c r="B204"/>
-      <c r="C204"/>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205"/>
+      <c r="C204" s="5"/>
+      <c r="D204" s="7"/>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="5"/>
       <c r="B205"/>
-      <c r="C205"/>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A206"/>
+      <c r="C205" s="5"/>
+      <c r="D205" s="7"/>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="5"/>
       <c r="B206"/>
-      <c r="C206"/>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207"/>
+      <c r="C206" s="5"/>
+      <c r="D206" s="7"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="5"/>
       <c r="B207"/>
-      <c r="C207"/>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208"/>
+      <c r="C207" s="5"/>
+      <c r="D207" s="7"/>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="5"/>
       <c r="B208"/>
-      <c r="C208"/>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209"/>
+      <c r="C208" s="5"/>
+      <c r="D208" s="7"/>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="5"/>
       <c r="B209"/>
-      <c r="C209"/>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210"/>
+      <c r="C209" s="5"/>
+      <c r="D209" s="7"/>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="5"/>
       <c r="B210"/>
-      <c r="C210"/>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211"/>
+      <c r="C210" s="5"/>
+      <c r="D210" s="7"/>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="5"/>
       <c r="B211"/>
-      <c r="C211"/>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212"/>
+      <c r="C211" s="5"/>
+      <c r="D211" s="7"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="5"/>
       <c r="B212"/>
-      <c r="C212"/>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213"/>
+      <c r="C212" s="5"/>
+      <c r="D212" s="7"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="5"/>
       <c r="B213"/>
-      <c r="C213"/>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214"/>
+      <c r="C213" s="5"/>
+      <c r="D213" s="7"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="5"/>
       <c r="B214"/>
-      <c r="C214"/>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215"/>
+      <c r="C214" s="5"/>
+      <c r="D214" s="7"/>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="5"/>
       <c r="B215"/>
-      <c r="C215"/>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216"/>
+      <c r="C215" s="5"/>
+      <c r="D215" s="7"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="5"/>
       <c r="B216"/>
-      <c r="C216"/>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217"/>
+      <c r="C216" s="5"/>
+      <c r="D216" s="7"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="5"/>
       <c r="B217"/>
-      <c r="C217"/>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218"/>
-      <c r="B218"/>
-      <c r="C218"/>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A219"/>
-      <c r="B219"/>
-      <c r="C219"/>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220"/>
-      <c r="B220"/>
-      <c r="C220"/>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221"/>
-      <c r="B221"/>
-      <c r="C221"/>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222"/>
-      <c r="B222"/>
-      <c r="C222"/>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A223"/>
-      <c r="B223"/>
-      <c r="C223"/>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A224"/>
-      <c r="B224"/>
-      <c r="C224"/>
+      <c r="C217" s="3"/>
+      <c r="D217" s="7"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="3"/>
+      <c r="B218" s="3"/>
+      <c r="C218" s="3"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="4"/>
+      <c r="B219" s="4"/>
+      <c r="C219" s="4"/>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" s="4"/>
+      <c r="B220" s="4"/>
+      <c r="C220" s="4"/>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="4"/>
+      <c r="B221" s="4"/>
+      <c r="C221" s="4"/>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="4"/>
+      <c r="B222" s="4"/>
+      <c r="C222" s="4"/>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="4"/>
+      <c r="B223" s="4"/>
+      <c r="C223" s="4"/>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="4"/>
+      <c r="B224" s="4"/>
+      <c r="C224" s="4"/>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225"/>
-      <c r="B225"/>
-      <c r="C225"/>
+      <c r="A225" s="4"/>
+      <c r="B225" s="4"/>
+      <c r="C225" s="4"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A226"/>
-      <c r="B226"/>
-      <c r="C226"/>
+      <c r="A226" s="4"/>
+      <c r="B226" s="4"/>
+      <c r="C226" s="4"/>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A227"/>
-      <c r="B227"/>
-      <c r="C227"/>
+      <c r="A227" s="4"/>
+      <c r="B227" s="4"/>
+      <c r="C227" s="4"/>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228"/>
-      <c r="B228"/>
-      <c r="C228"/>
+      <c r="A228" s="4"/>
+      <c r="B228" s="4"/>
+      <c r="C228" s="4"/>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229"/>
-      <c r="B229"/>
-      <c r="C229"/>
+      <c r="A229" s="4"/>
+      <c r="B229" s="4"/>
+      <c r="C229" s="4"/>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A230"/>
-      <c r="B230"/>
-      <c r="C230"/>
+      <c r="A230" s="4"/>
+      <c r="B230" s="4"/>
+      <c r="C230" s="4"/>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A231"/>
-      <c r="B231"/>
-      <c r="C231"/>
+      <c r="A231" s="4"/>
+      <c r="B231" s="4"/>
+      <c r="C231" s="4"/>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A232"/>
-      <c r="B232"/>
-      <c r="C232"/>
+      <c r="A232" s="4"/>
+      <c r="B232" s="4"/>
+      <c r="C232" s="4"/>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A233"/>
-      <c r="B233"/>
-      <c r="C233"/>
+      <c r="A233" s="4"/>
+      <c r="B233" s="4"/>
+      <c r="C233" s="4"/>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234"/>
-      <c r="B234"/>
-      <c r="C234"/>
+      <c r="A234" s="4"/>
+      <c r="B234" s="4"/>
+      <c r="C234" s="4"/>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A235"/>
-      <c r="B235"/>
-      <c r="C235"/>
+      <c r="A235" s="4"/>
+      <c r="B235" s="4"/>
+      <c r="C235" s="4"/>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A236"/>
-      <c r="B236"/>
-      <c r="C236"/>
+      <c r="A236" s="4"/>
+      <c r="B236" s="4"/>
+      <c r="C236" s="4"/>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237"/>
-      <c r="B237"/>
-      <c r="C237"/>
+      <c r="A237" s="4"/>
+      <c r="B237" s="4"/>
+      <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238"/>
-      <c r="B238"/>
-      <c r="C238"/>
+      <c r="A238" s="4"/>
+      <c r="B238" s="4"/>
+      <c r="C238" s="4"/>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239"/>
-      <c r="B239"/>
-      <c r="C239"/>
+      <c r="A239" s="4"/>
+      <c r="B239" s="4"/>
+      <c r="C239" s="4"/>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240"/>
-      <c r="B240"/>
-      <c r="C240"/>
+      <c r="A240" s="4"/>
+      <c r="B240" s="4"/>
+      <c r="C240" s="4"/>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A241"/>
-      <c r="B241"/>
-      <c r="C241"/>
+      <c r="A241" s="4"/>
+      <c r="B241" s="4"/>
+      <c r="C241" s="4"/>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242"/>
-      <c r="B242"/>
-      <c r="C242"/>
+      <c r="A242" s="4"/>
+      <c r="B242" s="4"/>
+      <c r="C242" s="4"/>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243"/>
-      <c r="B243"/>
-      <c r="C243"/>
+      <c r="A243" s="4"/>
+      <c r="B243" s="4"/>
+      <c r="C243" s="4"/>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244"/>
-      <c r="B244"/>
-      <c r="C244"/>
+      <c r="A244" s="4"/>
+      <c r="B244" s="4"/>
+      <c r="C244" s="4"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245"/>
-      <c r="B245"/>
-      <c r="C245"/>
+      <c r="A245" s="4"/>
+      <c r="B245" s="4"/>
+      <c r="C245" s="4"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A246"/>
-      <c r="B246"/>
-      <c r="C246"/>
+      <c r="A246" s="4"/>
+      <c r="B246" s="4"/>
+      <c r="C246" s="4"/>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247"/>
-      <c r="B247"/>
-      <c r="C247"/>
+      <c r="A247" s="4"/>
+      <c r="B247" s="4"/>
+      <c r="C247" s="4"/>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A248"/>
-      <c r="B248"/>
-      <c r="C248"/>
+      <c r="A248" s="4"/>
+      <c r="B248" s="4"/>
+      <c r="C248" s="4"/>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A249"/>
-      <c r="B249"/>
-      <c r="C249"/>
+      <c r="A249" s="4"/>
+      <c r="B249" s="4"/>
+      <c r="C249" s="4"/>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A250"/>
-      <c r="B250"/>
-      <c r="C250"/>
+      <c r="A250" s="4"/>
+      <c r="B250" s="4"/>
+      <c r="C250" s="4"/>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251"/>
-      <c r="B251"/>
-      <c r="C251"/>
+      <c r="A251" s="4"/>
+      <c r="B251" s="4"/>
+      <c r="C251" s="4"/>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252"/>
-      <c r="B252"/>
-      <c r="C252"/>
+      <c r="A252" s="4"/>
+      <c r="B252" s="4"/>
+      <c r="C252" s="4"/>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253"/>
-      <c r="B253"/>
-      <c r="C253"/>
+      <c r="A253" s="4"/>
+      <c r="B253" s="4"/>
+      <c r="C253" s="4"/>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A254"/>
-      <c r="B254"/>
-      <c r="C254"/>
+      <c r="A254" s="4"/>
+      <c r="B254" s="4"/>
+      <c r="C254" s="4"/>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A255"/>
-      <c r="B255"/>
-      <c r="C255"/>
+      <c r="A255" s="4"/>
+      <c r="B255" s="4"/>
+      <c r="C255" s="4"/>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A256"/>
-      <c r="B256"/>
-      <c r="C256"/>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257"/>
-      <c r="B257"/>
-      <c r="C257"/>
+      <c r="A256" s="4"/>
+      <c r="B256" s="4"/>
+      <c r="C256" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1668,7 +1912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>